<commit_message>
Added full dataset and corrected nats
</commit_message>
<xml_diff>
--- a/nationalities.xlsx
+++ b/nationalities.xlsx
@@ -11,7 +11,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+  <si>
+    <t>Nationalities</t>
+  </si>
+  <si>
+    <t>Counts</t>
+  </si>
   <si>
     <r>
       <rPr>
@@ -46,15 +52,7 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="Arial, &quot;Helvetica Neue&quot;, Helvetica, sans-serif"/>
-        <color rgb="FF1155CC"/>
-        <sz val="9.0"/>
-        <u/>
-      </rPr>
-      <t>Dutch'</t>
-    </r>
+    <t>Dutch</t>
   </si>
   <si>
     <r>
@@ -240,6 +238,17 @@
         <sz val="9.0"/>
         <u/>
       </rPr>
+      <t>Clevelander</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial, &quot;Helvetica Neue&quot;, Helvetica, sans-serif"/>
+        <color rgb="FF1155CC"/>
+        <sz val="9.0"/>
+        <u/>
+      </rPr>
       <t>Liégeois</t>
     </r>
   </si>
@@ -251,17 +260,6 @@
         <sz val="9.0"/>
         <u/>
       </rPr>
-      <t>Clevelander</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial, &quot;Helvetica Neue&quot;, Helvetica, sans-serif"/>
-        <color rgb="FF1155CC"/>
-        <sz val="9.0"/>
-        <u/>
-      </rPr>
       <t>Utrechter</t>
     </r>
   </si>
@@ -482,6 +480,17 @@
         <sz val="9.0"/>
         <u/>
       </rPr>
+      <t>Roman</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial, &quot;Helvetica Neue&quot;, Helvetica, sans-serif"/>
+        <color rgb="FF1155CC"/>
+        <sz val="9.0"/>
+        <u/>
+      </rPr>
       <t>Ferrarese</t>
     </r>
   </si>
@@ -493,17 +502,6 @@
         <sz val="9.0"/>
         <u/>
       </rPr>
-      <t>Roman</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial, &quot;Helvetica Neue&quot;, Helvetica, sans-serif"/>
-        <color rgb="FF1155CC"/>
-        <sz val="9.0"/>
-        <u/>
-      </rPr>
       <t>Lorrainer</t>
     </r>
   </si>
@@ -607,15 +605,7 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="Arial, &quot;Helvetica Neue&quot;, Helvetica, sans-serif"/>
-        <color rgb="FF1155CC"/>
-        <sz val="9.0"/>
-        <u/>
-      </rPr>
-      <t>Indian'</t>
-    </r>
+    <t>Indian</t>
   </si>
   <si>
     <r>
@@ -684,15 +674,7 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="Arial, &quot;Helvetica Neue&quot;, Helvetica, sans-serif"/>
-        <color rgb="FF1155CC"/>
-        <sz val="9.0"/>
-        <u/>
-      </rPr>
-      <t>Northern man'</t>
-    </r>
+    <t>Northern man</t>
   </si>
   <si>
     <r>
@@ -703,17 +685,6 @@
         <u/>
       </rPr>
       <t>Armagnac</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial, &quot;Helvetica Neue&quot;, Helvetica, sans-serif"/>
-        <color rgb="FF1155CC"/>
-        <sz val="9.0"/>
-        <u/>
-      </rPr>
-      <t>Basque</t>
     </r>
   </si>
   <si>
@@ -732,12 +703,22 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="9.0"/>
+      <color rgb="FF262626"/>
+      <name val="Arial"/>
     </font>
     <font>
       <u/>
@@ -746,8 +727,9 @@
       <name val="Arial"/>
     </font>
     <font>
+      <u/>
       <sz val="9.0"/>
-      <color rgb="FF262626"/>
+      <color rgb="FF1155CC"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -782,17 +764,29 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="top"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="top"/>
     </xf>
-    <xf quotePrefix="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="top"/>
+    </xf>
+    <xf quotePrefix="1" borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="top"/>
+    </xf>
+    <xf quotePrefix="1" borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1015,590 +1009,593 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2">
-        <v>4568.0</v>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4">
+        <v>4560.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="4">
         <v>3361.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2">
-        <v>2173.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2">
-        <v>2163.0</v>
+        <v>4</v>
+      </c>
+      <c r="B4" s="4">
+        <v>2173.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2">
+      <c r="A5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="4">
+        <v>2161.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="4">
         <v>2019.0</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2">
+    <row r="7">
+      <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="4">
         <v>1321.0</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2">
-        <v>1162.0</v>
-      </c>
-    </row>
     <row r="8">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2">
+      <c r="A8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1161.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="4">
         <v>775.0</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2">
+    <row r="10">
+      <c r="A10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="4">
         <v>745.0</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2">
+    <row r="11">
+      <c r="A11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="4">
         <v>665.0</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2">
-        <v>529.0</v>
-      </c>
-    </row>
     <row r="12">
-      <c r="A12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="2">
-        <v>384.0</v>
+      <c r="A12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="4">
+        <v>528.0</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2">
+      <c r="A13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="4">
+        <v>383.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="4">
         <v>377.0</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="2">
+    <row r="15">
+      <c r="A15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="4">
         <v>281.0</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="2">
-        <v>265.0</v>
-      </c>
-    </row>
     <row r="16">
-      <c r="A16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="2">
-        <v>259.0</v>
+      <c r="A16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="4">
+        <v>263.0</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="2">
+      <c r="A17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="4">
+        <v>258.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="4">
         <v>249.0</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="2">
+    <row r="19">
+      <c r="A19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="4">
         <v>242.0</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="2">
+    <row r="20">
+      <c r="A20" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="4">
         <v>213.0</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="2">
+    <row r="21">
+      <c r="A21" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="4">
         <v>161.0</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="2">
-        <v>128.0</v>
-      </c>
-    </row>
     <row r="22">
-      <c r="A22" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="2">
+      <c r="A22" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="4">
         <v>127.0</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" s="2">
+      <c r="A23" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="4">
+        <v>127.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="4">
         <v>94.0</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" s="2">
+    <row r="25">
+      <c r="A25" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="4">
         <v>88.0</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" s="2">
+    <row r="26">
+      <c r="A26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="4">
         <v>80.0</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26" s="2">
+    <row r="27">
+      <c r="A27" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="4">
         <v>67.0</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B27" s="2">
+    <row r="28">
+      <c r="A28" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="4">
         <v>60.0</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B28" s="2">
+    <row r="29">
+      <c r="A29" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="4">
         <v>56.0</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29" s="2">
-        <v>53.0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30" s="2">
+        <v>30</v>
+      </c>
+      <c r="B30" s="4">
+        <v>53.0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="4">
         <v>52.0</v>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B31" s="2">
+    <row r="32">
+      <c r="A32" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="4">
         <v>43.0</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B32" s="2">
+    <row r="33">
+      <c r="A33" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="4">
         <v>38.0</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B33" s="2">
-        <v>38.0</v>
-      </c>
-    </row>
     <row r="34">
-      <c r="A34" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B34" s="2">
+      <c r="A34" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="4">
+        <v>37.0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="4">
         <v>33.0</v>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B35" s="2">
+    <row r="36">
+      <c r="A36" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" s="4">
         <v>21.0</v>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B36" s="2">
+    <row r="37">
+      <c r="A37" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="4">
         <v>21.0</v>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B37" s="2">
+    <row r="38">
+      <c r="A38" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="4">
         <v>19.0</v>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B38" s="2">
+    <row r="39">
+      <c r="A39" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" s="4">
         <v>18.0</v>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B39" s="2">
+    <row r="40">
+      <c r="A40" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" s="4">
         <v>15.0</v>
       </c>
     </row>
-    <row r="40">
-      <c r="A40" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B40" s="2">
+    <row r="41">
+      <c r="A41" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="4">
         <v>11.0</v>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B41" s="2">
+    <row r="42">
+      <c r="A42" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" s="4">
         <v>11.0</v>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B42" s="2">
+    <row r="43">
+      <c r="A43" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43" s="4">
         <v>8.0</v>
       </c>
     </row>
-    <row r="43">
-      <c r="A43" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B43" s="2">
+    <row r="44">
+      <c r="A44" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B44" s="4">
         <v>8.0</v>
       </c>
     </row>
-    <row r="44">
-      <c r="A44" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B44" s="2">
-        <v>8.0</v>
-      </c>
-    </row>
     <row r="45">
-      <c r="A45" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B45" s="2">
+      <c r="A45" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B45" s="4">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B46" s="4">
         <v>6.0</v>
       </c>
     </row>
-    <row r="46">
-      <c r="A46" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B46" s="2">
+    <row r="47">
+      <c r="A47" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47" s="4">
         <v>6.0</v>
       </c>
     </row>
-    <row r="47">
-      <c r="A47" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B47" s="2">
+    <row r="48">
+      <c r="A48" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B48" s="4">
         <v>6.0</v>
       </c>
     </row>
-    <row r="48">
-      <c r="A48" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B48" s="2">
+    <row r="49">
+      <c r="A49" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B49" s="4">
         <v>6.0</v>
       </c>
     </row>
-    <row r="49">
-      <c r="A49" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B49" s="2">
+    <row r="50">
+      <c r="A50" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B50" s="4">
         <v>5.0</v>
       </c>
     </row>
-    <row r="50">
-      <c r="A50" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B50" s="2">
+    <row r="51">
+      <c r="A51" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B51" s="4">
         <v>5.0</v>
       </c>
     </row>
-    <row r="51">
-      <c r="A51" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B51" s="2">
+    <row r="52">
+      <c r="A52" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B52" s="4">
         <v>5.0</v>
       </c>
     </row>
-    <row r="52">
-      <c r="A52" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B52" s="2">
+    <row r="53">
+      <c r="A53" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B53" s="4">
         <v>4.0</v>
       </c>
     </row>
-    <row r="53">
-      <c r="A53" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B53" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
     <row r="54">
-      <c r="A54" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B54" s="2">
+      <c r="A54" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B54" s="4">
         <v>4.0</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B55" s="2">
+        <v>55</v>
+      </c>
+      <c r="B55" s="4">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B56" s="4">
         <v>3.0</v>
       </c>
     </row>
-    <row r="56">
-      <c r="A56" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B56" s="2">
+    <row r="57">
+      <c r="A57" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B57" s="4">
         <v>3.0</v>
       </c>
     </row>
-    <row r="57">
-      <c r="A57" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B57" s="2">
+    <row r="58">
+      <c r="A58" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B58" s="4">
         <v>3.0</v>
       </c>
     </row>
-    <row r="58">
-      <c r="A58" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B58" s="2">
+    <row r="59">
+      <c r="A59" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B59" s="4">
         <v>3.0</v>
       </c>
     </row>
-    <row r="59">
-      <c r="A59" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B59" s="2">
+    <row r="60">
+      <c r="A60" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B60" s="4">
         <v>3.0</v>
       </c>
     </row>
-    <row r="60">
-      <c r="A60" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B60" s="2">
-        <v>2.0</v>
-      </c>
-    </row>
     <row r="61">
-      <c r="A61" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B61" s="2">
+      <c r="A61" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B61" s="4">
         <v>2.0</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B62" s="2">
+        <v>62</v>
+      </c>
+      <c r="B62" s="4">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B63" s="4">
         <v>1.0</v>
       </c>
     </row>
-    <row r="63">
-      <c r="A63" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B63" s="2">
+    <row r="64">
+      <c r="A64" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B64" s="4">
         <v>1.0</v>
       </c>
     </row>
-    <row r="64">
-      <c r="A64" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B64" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
     <row r="65">
-      <c r="A65" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B65" s="2">
-        <v>41700.0</v>
-      </c>
+      <c r="A65" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B65" s="4">
+        <v>41366.0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="7"/>
+      <c r="B66" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="A1"/>
-    <hyperlink r:id="rId2" ref="A2"/>
-    <hyperlink r:id="rId3" ref="A3"/>
-    <hyperlink r:id="rId4" ref="A4"/>
-    <hyperlink r:id="rId5" ref="A5"/>
-    <hyperlink r:id="rId6" ref="A6"/>
-    <hyperlink r:id="rId7" ref="A7"/>
-    <hyperlink r:id="rId8" ref="A8"/>
-    <hyperlink r:id="rId9" ref="A9"/>
-    <hyperlink r:id="rId10" ref="A10"/>
-    <hyperlink r:id="rId11" ref="A11"/>
-    <hyperlink r:id="rId12" ref="A12"/>
-    <hyperlink r:id="rId13" ref="A13"/>
-    <hyperlink r:id="rId14" ref="A14"/>
-    <hyperlink r:id="rId15" ref="A15"/>
-    <hyperlink r:id="rId16" ref="A16"/>
-    <hyperlink r:id="rId17" ref="A17"/>
-    <hyperlink r:id="rId18" ref="A18"/>
-    <hyperlink r:id="rId19" ref="A19"/>
-    <hyperlink r:id="rId20" ref="A20"/>
-    <hyperlink r:id="rId21" ref="A21"/>
-    <hyperlink r:id="rId22" ref="A22"/>
-    <hyperlink r:id="rId23" ref="A23"/>
-    <hyperlink r:id="rId24" ref="A24"/>
-    <hyperlink r:id="rId25" ref="A25"/>
-    <hyperlink r:id="rId26" ref="A26"/>
-    <hyperlink r:id="rId27" ref="A27"/>
-    <hyperlink r:id="rId28" ref="A28"/>
-    <hyperlink r:id="rId29" ref="A29"/>
-    <hyperlink r:id="rId30" ref="A30"/>
-    <hyperlink r:id="rId31" ref="A31"/>
-    <hyperlink r:id="rId32" ref="A32"/>
-    <hyperlink r:id="rId33" ref="A33"/>
-    <hyperlink r:id="rId34" ref="A34"/>
-    <hyperlink r:id="rId35" ref="A35"/>
-    <hyperlink r:id="rId36" ref="A36"/>
-    <hyperlink r:id="rId37" ref="A37"/>
-    <hyperlink r:id="rId38" ref="A38"/>
-    <hyperlink r:id="rId39" ref="A39"/>
-    <hyperlink r:id="rId40" ref="A40"/>
-    <hyperlink r:id="rId41" ref="A41"/>
-    <hyperlink r:id="rId42" ref="A42"/>
-    <hyperlink r:id="rId43" ref="A43"/>
-    <hyperlink r:id="rId44" ref="A44"/>
-    <hyperlink r:id="rId45" ref="A45"/>
-    <hyperlink r:id="rId46" ref="A46"/>
-    <hyperlink r:id="rId47" ref="A47"/>
-    <hyperlink r:id="rId48" ref="A48"/>
-    <hyperlink r:id="rId49" ref="A49"/>
-    <hyperlink r:id="rId50" ref="A50"/>
-    <hyperlink r:id="rId51" ref="A51"/>
-    <hyperlink r:id="rId52" ref="A52"/>
-    <hyperlink r:id="rId53" ref="A53"/>
-    <hyperlink r:id="rId54" ref="A54"/>
-    <hyperlink r:id="rId55" ref="A55"/>
-    <hyperlink r:id="rId56" ref="A56"/>
-    <hyperlink r:id="rId57" ref="A57"/>
-    <hyperlink r:id="rId58" ref="A58"/>
-    <hyperlink r:id="rId59" ref="A59"/>
-    <hyperlink r:id="rId60" ref="A60"/>
-    <hyperlink r:id="rId61" ref="A61"/>
-    <hyperlink r:id="rId62" ref="A62"/>
-    <hyperlink r:id="rId63" ref="A63"/>
-    <hyperlink r:id="rId64" ref="A64"/>
-    <hyperlink r:id="rId65" ref="A65"/>
+    <hyperlink r:id="rId1" ref="A2"/>
+    <hyperlink r:id="rId2" ref="A3"/>
+    <hyperlink r:id="rId3" ref="A4"/>
+    <hyperlink r:id="rId4" ref="A5"/>
+    <hyperlink r:id="rId5" ref="A6"/>
+    <hyperlink r:id="rId6" ref="A7"/>
+    <hyperlink r:id="rId7" ref="A8"/>
+    <hyperlink r:id="rId8" ref="A9"/>
+    <hyperlink r:id="rId9" ref="A10"/>
+    <hyperlink r:id="rId10" ref="A11"/>
+    <hyperlink r:id="rId11" ref="A12"/>
+    <hyperlink r:id="rId12" ref="A13"/>
+    <hyperlink r:id="rId13" ref="A14"/>
+    <hyperlink r:id="rId14" ref="A15"/>
+    <hyperlink r:id="rId15" ref="A16"/>
+    <hyperlink r:id="rId16" ref="A17"/>
+    <hyperlink r:id="rId17" ref="A18"/>
+    <hyperlink r:id="rId18" ref="A19"/>
+    <hyperlink r:id="rId19" ref="A20"/>
+    <hyperlink r:id="rId20" ref="A21"/>
+    <hyperlink r:id="rId21" ref="A22"/>
+    <hyperlink r:id="rId22" ref="A23"/>
+    <hyperlink r:id="rId23" ref="A24"/>
+    <hyperlink r:id="rId24" ref="A25"/>
+    <hyperlink r:id="rId25" ref="A26"/>
+    <hyperlink r:id="rId26" ref="A27"/>
+    <hyperlink r:id="rId27" ref="A28"/>
+    <hyperlink r:id="rId28" ref="A29"/>
+    <hyperlink r:id="rId29" ref="A30"/>
+    <hyperlink r:id="rId30" ref="A31"/>
+    <hyperlink r:id="rId31" ref="A32"/>
+    <hyperlink r:id="rId32" ref="A33"/>
+    <hyperlink r:id="rId33" ref="A34"/>
+    <hyperlink r:id="rId34" ref="A35"/>
+    <hyperlink r:id="rId35" ref="A36"/>
+    <hyperlink r:id="rId36" ref="A37"/>
+    <hyperlink r:id="rId37" ref="A38"/>
+    <hyperlink r:id="rId38" ref="A39"/>
+    <hyperlink r:id="rId39" ref="A40"/>
+    <hyperlink r:id="rId40" ref="A41"/>
+    <hyperlink r:id="rId41" ref="A42"/>
+    <hyperlink r:id="rId42" ref="A43"/>
+    <hyperlink r:id="rId43" ref="A44"/>
+    <hyperlink r:id="rId44" ref="A45"/>
+    <hyperlink r:id="rId45" ref="A46"/>
+    <hyperlink r:id="rId46" ref="A47"/>
+    <hyperlink r:id="rId47" ref="A48"/>
+    <hyperlink r:id="rId48" ref="A49"/>
+    <hyperlink r:id="rId49" ref="A50"/>
+    <hyperlink r:id="rId50" ref="A51"/>
+    <hyperlink r:id="rId51" ref="A52"/>
+    <hyperlink r:id="rId52" ref="A53"/>
+    <hyperlink r:id="rId53" ref="A54"/>
+    <hyperlink r:id="rId54" ref="A55"/>
+    <hyperlink r:id="rId55" ref="A56"/>
+    <hyperlink r:id="rId56" ref="A57"/>
+    <hyperlink r:id="rId57" ref="A58"/>
+    <hyperlink r:id="rId58" ref="A59"/>
+    <hyperlink r:id="rId59" ref="A60"/>
+    <hyperlink r:id="rId60" ref="A61"/>
+    <hyperlink r:id="rId61" ref="A62"/>
+    <hyperlink r:id="rId62" ref="A63"/>
+    <hyperlink r:id="rId63" ref="A64"/>
+    <hyperlink r:id="rId64" ref="A65"/>
   </hyperlinks>
-  <drawing r:id="rId66"/>
+  <drawing r:id="rId65"/>
 </worksheet>
 </file>
</xml_diff>